<commit_message>
added data for choropleth
</commit_message>
<xml_diff>
--- a/data/2016 Sales, Manufacturing Workbook.xlsx
+++ b/data/2016 Sales, Manufacturing Workbook.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dieterholger/Desktop/Git/US-Gun-Manufacturing-Interactive/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA38DC98-2E78-2749-AD67-BCEDBF561468}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8E2433-AE85-1A4F-BA54-8935F1FCFB2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2016 State Manufacturing vs Che" sheetId="1" r:id="rId1"/>
+    <sheet name="2016 State Checks vs Manufactur" sheetId="1" r:id="rId1"/>
     <sheet name="Estimated Sales vs Manufacturin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
@@ -1298,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -3911,9 +3911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed spell of Mississippi
</commit_message>
<xml_diff>
--- a/data/2016 Sales, Manufacturing Workbook.xlsx
+++ b/data/2016 Sales, Manufacturing Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dieterholger/Desktop/Git/US-Gun-Manufacturing-Interactive/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8E2433-AE85-1A4F-BA54-8935F1FCFB2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9F00E2-DF1E-F444-AF86-5198E10B5BC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016 State Checks vs Manufactur" sheetId="1" r:id="rId1"/>
@@ -444,10 +444,10 @@
     <t>Wyoming</t>
   </si>
   <si>
-    <t>Mississipi</t>
-  </si>
-  <si>
     <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
   </si>
 </sst>
 </file>
@@ -1298,9 +1298,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="25" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
@@ -3257,7 +3257,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B40" t="s">
         <v>64</v>
@@ -3911,9 +3911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3999,19 +3999,19 @@
         <v>6545</v>
       </c>
       <c r="H2">
-        <f>(E2*1.1)</f>
+        <f t="shared" ref="H2:H33" si="0">(E2*1.1)</f>
         <v>168435.30000000002</v>
       </c>
       <c r="I2">
-        <f>(F2*1.1)</f>
+        <f t="shared" ref="I2:I33" si="1">(F2*1.1)</f>
         <v>134159.30000000002</v>
       </c>
       <c r="J2">
-        <f>(G2*2)</f>
+        <f t="shared" ref="J2:J38" si="2">(G2*2)</f>
         <v>13090</v>
       </c>
       <c r="K2">
-        <f>SUM(H2:J2)</f>
+        <f t="shared" ref="K2:K33" si="3">SUM(H2:J2)</f>
         <v>315684.60000000003</v>
       </c>
       <c r="L2">
@@ -4056,19 +4056,19 @@
         <v>2316</v>
       </c>
       <c r="H3">
-        <f>(E3*1.1)</f>
+        <f t="shared" si="0"/>
         <v>41240.100000000006</v>
       </c>
       <c r="I3">
-        <f>(F3*1.1)</f>
+        <f t="shared" si="1"/>
         <v>40575.700000000004</v>
       </c>
       <c r="J3">
-        <f>(G3*2)</f>
+        <f t="shared" si="2"/>
         <v>4632</v>
       </c>
       <c r="K3">
-        <f>SUM(H3:J3)</f>
+        <f t="shared" si="3"/>
         <v>86447.800000000017</v>
       </c>
       <c r="L3">
@@ -4113,19 +4113,19 @@
         <v>7908</v>
       </c>
       <c r="H4">
-        <f>(E4*1.1)</f>
+        <f t="shared" si="0"/>
         <v>183462.40000000002</v>
       </c>
       <c r="I4">
-        <f>(F4*1.1)</f>
+        <f t="shared" si="1"/>
         <v>119886.8</v>
       </c>
       <c r="J4">
-        <f>(G4*2)</f>
+        <f t="shared" si="2"/>
         <v>15816</v>
       </c>
       <c r="K4">
-        <f>SUM(H4:J4)</f>
+        <f t="shared" si="3"/>
         <v>319165.2</v>
       </c>
       <c r="L4">
@@ -4170,19 +4170,19 @@
         <v>4400</v>
       </c>
       <c r="H5">
-        <f>(E5*1.1)</f>
+        <f t="shared" si="0"/>
         <v>88268.400000000009</v>
       </c>
       <c r="I5">
-        <f>(F5*1.1)</f>
+        <f t="shared" si="1"/>
         <v>90332.000000000015</v>
       </c>
       <c r="J5">
-        <f>(G5*2)</f>
+        <f t="shared" si="2"/>
         <v>8800</v>
       </c>
       <c r="K5">
-        <f>SUM(H5:J5)</f>
+        <f t="shared" si="3"/>
         <v>187400.40000000002</v>
       </c>
       <c r="L5">
@@ -4227,19 +4227,19 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <f>(E6*1.1)</f>
+        <f t="shared" si="0"/>
         <v>616390.5</v>
       </c>
       <c r="I6">
-        <f>(F6*1.1)</f>
+        <f t="shared" si="1"/>
         <v>610005</v>
       </c>
       <c r="J6">
-        <f>(G6*2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K6">
-        <f>SUM(H6:J6)</f>
+        <f t="shared" si="3"/>
         <v>1226395.5</v>
       </c>
       <c r="L6">
@@ -4284,19 +4284,19 @@
         <v>14293</v>
       </c>
       <c r="H7">
-        <f>(E7*1.1)</f>
+        <f t="shared" si="0"/>
         <v>266752.2</v>
       </c>
       <c r="I7">
-        <f>(F7*1.1)</f>
+        <f t="shared" si="1"/>
         <v>198028.6</v>
       </c>
       <c r="J7">
-        <f>(G7*2)</f>
+        <f t="shared" si="2"/>
         <v>28586</v>
       </c>
       <c r="K7">
-        <f>SUM(H7:J7)</f>
+        <f t="shared" si="3"/>
         <v>493366.80000000005</v>
       </c>
       <c r="L7">
@@ -4341,19 +4341,19 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <f>(E8*1.1)</f>
+        <f t="shared" si="0"/>
         <v>134612.5</v>
       </c>
       <c r="I8">
-        <f>(F8*1.1)</f>
+        <f t="shared" si="1"/>
         <v>48194.3</v>
       </c>
       <c r="J8">
-        <f>(G8*2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K8">
-        <f>SUM(H8:J8)</f>
+        <f t="shared" si="3"/>
         <v>182806.8</v>
       </c>
       <c r="L8">
@@ -4398,19 +4398,19 @@
         <v>1034</v>
       </c>
       <c r="H9">
-        <f>(E9*1.1)</f>
+        <f t="shared" si="0"/>
         <v>28131.4</v>
       </c>
       <c r="I9">
-        <f>(F9*1.1)</f>
+        <f t="shared" si="1"/>
         <v>23920.600000000002</v>
       </c>
       <c r="J9">
-        <f>(G9*2)</f>
+        <f t="shared" si="2"/>
         <v>2068</v>
       </c>
       <c r="K9">
-        <f>SUM(H9:J9)</f>
+        <f t="shared" si="3"/>
         <v>54120</v>
       </c>
       <c r="L9">
@@ -4455,19 +4455,19 @@
         <v>25142</v>
       </c>
       <c r="H10">
-        <f>(E10*1.1)</f>
+        <f t="shared" si="0"/>
         <v>728538.8</v>
       </c>
       <c r="I10">
-        <f>(F10*1.1)</f>
+        <f t="shared" si="1"/>
         <v>347855.2</v>
       </c>
       <c r="J10">
-        <f>(G10*2)</f>
+        <f t="shared" si="2"/>
         <v>50284</v>
       </c>
       <c r="K10">
-        <f>SUM(H10:J10)</f>
+        <f t="shared" si="3"/>
         <v>1126678</v>
       </c>
       <c r="L10">
@@ -4512,19 +4512,19 @@
         <v>7478</v>
       </c>
       <c r="H11">
-        <f>(E11*1.1)</f>
+        <f t="shared" si="0"/>
         <v>214280.00000000003</v>
       </c>
       <c r="I11">
-        <f>(F11*1.1)</f>
+        <f t="shared" si="1"/>
         <v>141104.70000000001</v>
       </c>
       <c r="J11">
-        <f>(G11*2)</f>
+        <f t="shared" si="2"/>
         <v>14956</v>
       </c>
       <c r="K11">
-        <f>SUM(H11:J11)</f>
+        <f t="shared" si="3"/>
         <v>370340.70000000007</v>
       </c>
       <c r="L11">
@@ -4569,19 +4569,19 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <f>(E12*1.1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I12">
-        <f>(F12*1.1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J12">
-        <f>(G12*2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K12">
-        <f>SUM(H12:J12)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L12">
@@ -4626,19 +4626,19 @@
         <v>2406</v>
       </c>
       <c r="H13">
-        <f>(E13*1.1)</f>
+        <f t="shared" si="0"/>
         <v>51175.3</v>
       </c>
       <c r="I13">
-        <f>(F13*1.1)</f>
+        <f t="shared" si="1"/>
         <v>61150.100000000006</v>
       </c>
       <c r="J13">
-        <f>(G13*2)</f>
+        <f t="shared" si="2"/>
         <v>4812</v>
       </c>
       <c r="K13">
-        <f>SUM(H13:J13)</f>
+        <f t="shared" si="3"/>
         <v>117137.40000000001</v>
       </c>
       <c r="L13">
@@ -4683,19 +4683,19 @@
         <v>12133</v>
       </c>
       <c r="H14">
-        <f>(E14*1.1)</f>
+        <f t="shared" si="0"/>
         <v>387652.10000000003</v>
       </c>
       <c r="I14">
-        <f>(F14*1.1)</f>
+        <f t="shared" si="1"/>
         <v>194980.50000000003</v>
       </c>
       <c r="J14">
-        <f>(G14*2)</f>
+        <f t="shared" si="2"/>
         <v>24266</v>
       </c>
       <c r="K14">
-        <f>SUM(H14:J14)</f>
+        <f t="shared" si="3"/>
         <v>606898.60000000009</v>
       </c>
       <c r="L14">
@@ -4740,19 +4740,19 @@
         <v>9082</v>
       </c>
       <c r="H15">
-        <f>(E15*1.1)</f>
+        <f t="shared" si="0"/>
         <v>306000.2</v>
       </c>
       <c r="I15">
-        <f>(F15*1.1)</f>
+        <f t="shared" si="1"/>
         <v>194939.80000000002</v>
       </c>
       <c r="J15">
-        <f>(G15*2)</f>
+        <f t="shared" si="2"/>
         <v>18164</v>
       </c>
       <c r="K15">
-        <f>SUM(H15:J15)</f>
+        <f t="shared" si="3"/>
         <v>519104</v>
       </c>
       <c r="L15">
@@ -4797,19 +4797,19 @@
         <v>70</v>
       </c>
       <c r="H16">
-        <f>(E16*1.1)</f>
+        <f t="shared" si="0"/>
         <v>3069.0000000000005</v>
       </c>
       <c r="I16">
-        <f>(F16*1.1)</f>
+        <f t="shared" si="1"/>
         <v>38779.4</v>
       </c>
       <c r="J16">
-        <f>(G16*2)</f>
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
       <c r="K16">
-        <f>SUM(H16:J16)</f>
+        <f t="shared" si="3"/>
         <v>41988.4</v>
       </c>
       <c r="L16">
@@ -4854,19 +4854,19 @@
         <v>4271</v>
       </c>
       <c r="H17">
-        <f>(E17*1.1)</f>
+        <f t="shared" si="0"/>
         <v>89227.6</v>
       </c>
       <c r="I17">
-        <f>(F17*1.1)</f>
+        <f t="shared" si="1"/>
         <v>81122.8</v>
       </c>
       <c r="J17">
-        <f>(G17*2)</f>
+        <f t="shared" si="2"/>
         <v>8542</v>
       </c>
       <c r="K17">
-        <f>SUM(H17:J17)</f>
+        <f t="shared" si="3"/>
         <v>178892.40000000002</v>
       </c>
       <c r="L17">
@@ -4911,19 +4911,19 @@
         <v>6943</v>
       </c>
       <c r="H18">
-        <f>(E18*1.1)</f>
+        <f t="shared" si="0"/>
         <v>154793.1</v>
       </c>
       <c r="I18">
-        <f>(F18*1.1)</f>
+        <f t="shared" si="1"/>
         <v>119933.00000000001</v>
       </c>
       <c r="J18">
-        <f>(G18*2)</f>
+        <f t="shared" si="2"/>
         <v>13886</v>
       </c>
       <c r="K18">
-        <f>SUM(H18:J18)</f>
+        <f t="shared" si="3"/>
         <v>288612.10000000003</v>
       </c>
       <c r="L18">
@@ -4968,19 +4968,19 @@
         <v>8609</v>
       </c>
       <c r="H19">
-        <f>(E19*1.1)</f>
+        <f t="shared" si="0"/>
         <v>188746.80000000002</v>
       </c>
       <c r="I19">
-        <f>(F19*1.1)</f>
+        <f t="shared" si="1"/>
         <v>153034.20000000001</v>
       </c>
       <c r="J19">
-        <f>(G19*2)</f>
+        <f t="shared" si="2"/>
         <v>17218</v>
       </c>
       <c r="K19">
-        <f>SUM(H19:J19)</f>
+        <f t="shared" si="3"/>
         <v>358999</v>
       </c>
       <c r="L19">
@@ -5025,19 +5025,19 @@
         <v>2458</v>
       </c>
       <c r="H20">
-        <f>(E20*1.1)</f>
+        <f t="shared" si="0"/>
         <v>53729.500000000007</v>
       </c>
       <c r="I20">
-        <f>(F20*1.1)</f>
+        <f t="shared" si="1"/>
         <v>51458.000000000007</v>
       </c>
       <c r="J20">
-        <f>(G20*2)</f>
+        <f t="shared" si="2"/>
         <v>4916</v>
       </c>
       <c r="K20">
-        <f>SUM(H20:J20)</f>
+        <f t="shared" si="3"/>
         <v>110103.50000000001</v>
       </c>
       <c r="L20">
@@ -5082,19 +5082,19 @@
         <v>337</v>
       </c>
       <c r="H21">
-        <f>(E21*1.1)</f>
+        <f t="shared" si="0"/>
         <v>57535.500000000007</v>
       </c>
       <c r="I21">
-        <f>(F21*1.1)</f>
+        <f t="shared" si="1"/>
         <v>79081.200000000012</v>
       </c>
       <c r="J21">
-        <f>(G21*2)</f>
+        <f t="shared" si="2"/>
         <v>674</v>
       </c>
       <c r="K21">
-        <f>SUM(H21:J21)</f>
+        <f t="shared" si="3"/>
         <v>137290.70000000001</v>
       </c>
       <c r="L21">
@@ -5139,19 +5139,19 @@
         <v>2480</v>
       </c>
       <c r="H22">
-        <f>(E22*1.1)</f>
+        <f t="shared" si="0"/>
         <v>83574.700000000012</v>
       </c>
       <c r="I22">
-        <f>(F22*1.1)</f>
+        <f t="shared" si="1"/>
         <v>46124.100000000006</v>
       </c>
       <c r="J22">
-        <f>(G22*2)</f>
+        <f t="shared" si="2"/>
         <v>4960</v>
       </c>
       <c r="K22">
-        <f>SUM(H22:J22)</f>
+        <f t="shared" si="3"/>
         <v>134658.80000000002</v>
       </c>
       <c r="L22">
@@ -5196,19 +5196,19 @@
         <v>2815</v>
       </c>
       <c r="H23">
-        <f>(E23*1.1)</f>
+        <f t="shared" si="0"/>
         <v>181365.80000000002</v>
       </c>
       <c r="I23">
-        <f>(F23*1.1)</f>
+        <f t="shared" si="1"/>
         <v>141997.90000000002</v>
       </c>
       <c r="J23">
-        <f>(G23*2)</f>
+        <f t="shared" si="2"/>
         <v>5630</v>
       </c>
       <c r="K23">
-        <f>SUM(H23:J23)</f>
+        <f t="shared" si="3"/>
         <v>328993.70000000007</v>
       </c>
       <c r="L23">
@@ -5253,19 +5253,19 @@
         <v>5046</v>
       </c>
       <c r="H24">
-        <f>(E24*1.1)</f>
+        <f t="shared" si="0"/>
         <v>147358.20000000001</v>
       </c>
       <c r="I24">
-        <f>(F24*1.1)</f>
+        <f t="shared" si="1"/>
         <v>157897.30000000002</v>
       </c>
       <c r="J24">
-        <f>(G24*2)</f>
+        <f t="shared" si="2"/>
         <v>10092</v>
       </c>
       <c r="K24">
-        <f>SUM(H24:J24)</f>
+        <f t="shared" si="3"/>
         <v>315347.5</v>
       </c>
       <c r="L24">
@@ -5289,7 +5289,7 @@
     </row>
     <row r="25" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
@@ -5310,19 +5310,19 @@
         <v>5263</v>
       </c>
       <c r="H25">
-        <f>(E25*1.1)</f>
+        <f t="shared" si="0"/>
         <v>130955.00000000001</v>
       </c>
       <c r="I25">
-        <f>(F25*1.1)</f>
+        <f t="shared" si="1"/>
         <v>102104.20000000001</v>
       </c>
       <c r="J25">
-        <f>(G25*2)</f>
+        <f t="shared" si="2"/>
         <v>10526</v>
       </c>
       <c r="K25">
-        <f>SUM(H25:J25)</f>
+        <f t="shared" si="3"/>
         <v>243585.2</v>
       </c>
       <c r="L25">
@@ -5367,19 +5367,19 @@
         <v>12753</v>
       </c>
       <c r="H26">
-        <f>(E26*1.1)</f>
+        <f t="shared" si="0"/>
         <v>302229.40000000002</v>
       </c>
       <c r="I26">
-        <f>(F26*1.1)</f>
+        <f t="shared" si="1"/>
         <v>222978.80000000002</v>
       </c>
       <c r="J26">
-        <f>(G26*2)</f>
+        <f t="shared" si="2"/>
         <v>25506</v>
       </c>
       <c r="K26">
-        <f>SUM(H26:J26)</f>
+        <f t="shared" si="3"/>
         <v>550714.20000000007</v>
       </c>
       <c r="L26">
@@ -5424,19 +5424,19 @@
         <v>2678</v>
       </c>
       <c r="H27">
-        <f>(E27*1.1)</f>
+        <f t="shared" si="0"/>
         <v>41301.700000000004</v>
       </c>
       <c r="I27">
-        <f>(F27*1.1)</f>
+        <f t="shared" si="1"/>
         <v>62517.4</v>
       </c>
       <c r="J27">
-        <f>(G27*2)</f>
+        <f t="shared" si="2"/>
         <v>5356</v>
       </c>
       <c r="K27">
-        <f>SUM(H27:J27)</f>
+        <f t="shared" si="3"/>
         <v>109175.1</v>
       </c>
       <c r="L27">
@@ -5481,19 +5481,19 @@
         <v>82</v>
       </c>
       <c r="H28">
-        <f>(E28*1.1)</f>
+        <f t="shared" si="0"/>
         <v>1888.7</v>
       </c>
       <c r="I28">
-        <f>(F28*1.1)</f>
+        <f t="shared" si="1"/>
         <v>29143.4</v>
       </c>
       <c r="J28">
-        <f>(G28*2)</f>
+        <f t="shared" si="2"/>
         <v>164</v>
       </c>
       <c r="K28">
-        <f>SUM(H28:J28)</f>
+        <f t="shared" si="3"/>
         <v>31196.100000000002</v>
       </c>
       <c r="L28">
@@ -5538,19 +5538,19 @@
         <v>3723</v>
       </c>
       <c r="H29">
-        <f>(E29*1.1)</f>
+        <f t="shared" si="0"/>
         <v>72773.8</v>
       </c>
       <c r="I29">
-        <f>(F29*1.1)</f>
+        <f t="shared" si="1"/>
         <v>41915.5</v>
       </c>
       <c r="J29">
-        <f>(G29*2)</f>
+        <f t="shared" si="2"/>
         <v>7446</v>
       </c>
       <c r="K29">
-        <f>SUM(H29:J29)</f>
+        <f t="shared" si="3"/>
         <v>122135.3</v>
       </c>
       <c r="L29">
@@ -5595,19 +5595,19 @@
         <v>55</v>
       </c>
       <c r="H30">
-        <f>(E30*1.1)</f>
+        <f t="shared" si="0"/>
         <v>75381.900000000009</v>
       </c>
       <c r="I30">
-        <f>(F30*1.1)</f>
+        <f t="shared" si="1"/>
         <v>49149.100000000006</v>
       </c>
       <c r="J30">
-        <f>(G30*2)</f>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="K30">
-        <f>SUM(H30:J30)</f>
+        <f t="shared" si="3"/>
         <v>124641.00000000001</v>
       </c>
       <c r="L30">
@@ -5652,19 +5652,19 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <f>(E31*1.1)</f>
+        <f t="shared" si="0"/>
         <v>77273.900000000009</v>
       </c>
       <c r="I31">
-        <f>(F31*1.1)</f>
+        <f t="shared" si="1"/>
         <v>54008.9</v>
       </c>
       <c r="J31">
-        <f>(G31*2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K31">
-        <f>SUM(H31:J31)</f>
+        <f t="shared" si="3"/>
         <v>131282.80000000002</v>
       </c>
       <c r="L31">
@@ -5709,19 +5709,19 @@
         <v>3732</v>
       </c>
       <c r="H32">
-        <f>(E32*1.1)</f>
+        <f t="shared" si="0"/>
         <v>76377.400000000009</v>
       </c>
       <c r="I32">
-        <f>(F32*1.1)</f>
+        <f t="shared" si="1"/>
         <v>61230.400000000001</v>
       </c>
       <c r="J32">
-        <f>(G32*2)</f>
+        <f t="shared" si="2"/>
         <v>7464</v>
       </c>
       <c r="K32">
-        <f>SUM(H32:J32)</f>
+        <f t="shared" si="3"/>
         <v>145071.80000000002</v>
       </c>
       <c r="L32">
@@ -5766,19 +5766,19 @@
         <v>2466</v>
       </c>
       <c r="H33">
-        <f>(E33*1.1)</f>
+        <f t="shared" si="0"/>
         <v>146613.5</v>
       </c>
       <c r="I33">
-        <f>(F33*1.1)</f>
+        <f t="shared" si="1"/>
         <v>217437.00000000003</v>
       </c>
       <c r="J33">
-        <f>(G33*2)</f>
+        <f t="shared" si="2"/>
         <v>4932</v>
       </c>
       <c r="K33">
-        <f>SUM(H33:J33)</f>
+        <f t="shared" si="3"/>
         <v>368982.5</v>
       </c>
       <c r="L33">
@@ -5823,19 +5823,19 @@
         <v>2812</v>
       </c>
       <c r="H34">
-        <f>(E34*1.1)</f>
+        <f t="shared" ref="H34:H52" si="4">(E34*1.1)</f>
         <v>18254.5</v>
       </c>
       <c r="I34">
-        <f>(F34*1.1)</f>
+        <f t="shared" ref="I34:I52" si="5">(F34*1.1)</f>
         <v>194610.90000000002</v>
       </c>
       <c r="J34">
-        <f>(G34*2)</f>
+        <f t="shared" si="2"/>
         <v>5624</v>
       </c>
       <c r="K34">
-        <f>SUM(H34:J34)</f>
+        <f t="shared" ref="K34:K65" si="6">SUM(H34:J34)</f>
         <v>218489.40000000002</v>
       </c>
       <c r="L34">
@@ -5880,19 +5880,19 @@
         <v>972</v>
       </c>
       <c r="H35">
-        <f>(E35*1.1)</f>
+        <f t="shared" si="4"/>
         <v>21972.5</v>
       </c>
       <c r="I35">
-        <f>(F35*1.1)</f>
+        <f t="shared" si="5"/>
         <v>37414.300000000003</v>
       </c>
       <c r="J35">
-        <f>(G35*2)</f>
+        <f t="shared" si="2"/>
         <v>1944</v>
       </c>
       <c r="K35">
-        <f>SUM(H35:J35)</f>
+        <f t="shared" si="6"/>
         <v>61330.8</v>
       </c>
       <c r="L35">
@@ -5937,19 +5937,19 @@
         <v>16333</v>
       </c>
       <c r="H36">
-        <f>(E36*1.1)</f>
+        <f t="shared" si="4"/>
         <v>434027.00000000006</v>
       </c>
       <c r="I36">
-        <f>(F36*1.1)</f>
+        <f t="shared" si="5"/>
         <v>268359.30000000005</v>
       </c>
       <c r="J36">
-        <f>(G36*2)</f>
+        <f t="shared" si="2"/>
         <v>32666</v>
       </c>
       <c r="K36">
-        <f>SUM(H36:J36)</f>
+        <f t="shared" si="6"/>
         <v>735052.3</v>
       </c>
       <c r="L36">
@@ -5994,19 +5994,19 @@
         <v>10661</v>
       </c>
       <c r="H37">
-        <f>(E37*1.1)</f>
+        <f t="shared" si="4"/>
         <v>182799.1</v>
       </c>
       <c r="I37">
-        <f>(F37*1.1)</f>
+        <f t="shared" si="5"/>
         <v>143565.40000000002</v>
       </c>
       <c r="J37">
-        <f>(G37*2)</f>
+        <f t="shared" si="2"/>
         <v>21322</v>
       </c>
       <c r="K37">
-        <f>SUM(H37:J37)</f>
+        <f t="shared" si="6"/>
         <v>347686.5</v>
       </c>
       <c r="L37">
@@ -6051,19 +6051,19 @@
         <v>0</v>
       </c>
       <c r="H38">
-        <f>(E38*1.1)</f>
+        <f t="shared" si="4"/>
         <v>196587.6</v>
       </c>
       <c r="I38">
-        <f>(F38*1.1)</f>
+        <f t="shared" si="5"/>
         <v>157331.90000000002</v>
       </c>
       <c r="J38">
-        <f>(G38*2)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K38">
-        <f>SUM(H38:J38)</f>
+        <f t="shared" si="6"/>
         <v>353919.5</v>
       </c>
       <c r="L38">
@@ -6108,15 +6108,15 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <f>(E39*1.1)</f>
+        <f t="shared" si="4"/>
         <v>706455.20000000007</v>
       </c>
       <c r="I39">
-        <f>(F39*1.1)</f>
+        <f t="shared" si="5"/>
         <v>173955.1</v>
       </c>
       <c r="K39">
-        <f>SUM(H39:J39)</f>
+        <f t="shared" si="6"/>
         <v>880410.3</v>
       </c>
       <c r="L39">
@@ -6140,7 +6140,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B40" t="s">
         <v>64</v>
@@ -6161,19 +6161,19 @@
         <v>275</v>
       </c>
       <c r="H40">
-        <f>(E40*1.1)</f>
+        <f t="shared" si="4"/>
         <v>14056.900000000001</v>
       </c>
       <c r="I40">
-        <f>(F40*1.1)</f>
+        <f t="shared" si="5"/>
         <v>2657.6000000000004</v>
       </c>
       <c r="J40">
-        <f>(G40*2)</f>
+        <f t="shared" ref="J40:J52" si="7">(G40*2)</f>
         <v>550</v>
       </c>
       <c r="K40">
-        <f>SUM(H40:J40)</f>
+        <f t="shared" si="6"/>
         <v>17264.5</v>
       </c>
       <c r="L40">
@@ -6209,19 +6209,19 @@
         <v>1999</v>
       </c>
       <c r="H41">
-        <f>(E41*1.1)</f>
+        <f t="shared" si="4"/>
         <v>15688.2</v>
       </c>
       <c r="I41">
-        <f>(F41*1.1)</f>
+        <f t="shared" si="5"/>
         <v>11224.400000000001</v>
       </c>
       <c r="J41">
-        <f>(G41*2)</f>
+        <f t="shared" si="7"/>
         <v>3998</v>
       </c>
       <c r="K41">
-        <f>SUM(H41:J41)</f>
+        <f t="shared" si="6"/>
         <v>30910.600000000002</v>
       </c>
       <c r="L41">
@@ -6266,19 +6266,19 @@
         <v>4490</v>
       </c>
       <c r="H42">
-        <f>(E42*1.1)</f>
+        <f t="shared" si="4"/>
         <v>145720.30000000002</v>
       </c>
       <c r="I42">
-        <f>(F42*1.1)</f>
+        <f t="shared" si="5"/>
         <v>96154.3</v>
       </c>
       <c r="J42">
-        <f>(G42*2)</f>
+        <f t="shared" si="7"/>
         <v>8980</v>
       </c>
       <c r="K42">
-        <f>SUM(H42:J42)</f>
+        <f t="shared" si="6"/>
         <v>250854.60000000003</v>
       </c>
       <c r="L42">
@@ -6323,19 +6323,19 @@
         <v>2184</v>
       </c>
       <c r="H43">
-        <f>(E43*1.1)</f>
+        <f t="shared" si="4"/>
         <v>40172</v>
       </c>
       <c r="I43">
-        <f>(F43*1.1)</f>
+        <f t="shared" si="5"/>
         <v>54474.200000000004</v>
       </c>
       <c r="J43">
-        <f>(G43*2)</f>
+        <f t="shared" si="7"/>
         <v>4368</v>
       </c>
       <c r="K43">
-        <f>SUM(H43:J43)</f>
+        <f t="shared" si="6"/>
         <v>99014.200000000012</v>
       </c>
       <c r="L43">
@@ -6380,19 +6380,19 @@
         <v>11092</v>
       </c>
       <c r="H44">
-        <f>(E44*1.1)</f>
+        <f t="shared" si="4"/>
         <v>351085.9</v>
       </c>
       <c r="I44">
-        <f>(F44*1.1)</f>
+        <f t="shared" si="5"/>
         <v>231177.1</v>
       </c>
       <c r="J44">
-        <f>(G44*2)</f>
+        <f t="shared" si="7"/>
         <v>22184</v>
       </c>
       <c r="K44">
-        <f>SUM(H44:J44)</f>
+        <f t="shared" si="6"/>
         <v>604447</v>
       </c>
       <c r="L44">
@@ -6437,19 +6437,19 @@
         <v>33102</v>
       </c>
       <c r="H45">
-        <f>(E45*1.1)</f>
+        <f t="shared" si="4"/>
         <v>701223.60000000009</v>
       </c>
       <c r="I45">
-        <f>(F45*1.1)</f>
+        <f t="shared" si="5"/>
         <v>529769.9</v>
       </c>
       <c r="J45">
-        <f>(G45*2)</f>
+        <f t="shared" si="7"/>
         <v>66204</v>
       </c>
       <c r="K45">
-        <f>SUM(H45:J45)</f>
+        <f t="shared" si="6"/>
         <v>1297197.5</v>
       </c>
       <c r="L45">
@@ -6494,19 +6494,19 @@
         <v>1191</v>
       </c>
       <c r="H46">
-        <f>(E46*1.1)</f>
+        <f t="shared" si="4"/>
         <v>52141.100000000006</v>
       </c>
       <c r="I46">
-        <f>(F46*1.1)</f>
+        <f t="shared" si="5"/>
         <v>59546.3</v>
       </c>
       <c r="J46">
-        <f>(G46*2)</f>
+        <f t="shared" si="7"/>
         <v>2382</v>
       </c>
       <c r="K46">
-        <f>SUM(H46:J46)</f>
+        <f t="shared" si="6"/>
         <v>114069.40000000001</v>
       </c>
       <c r="L46">
@@ -6551,19 +6551,19 @@
         <v>885</v>
       </c>
       <c r="H47">
-        <f>(E47*1.1)</f>
+        <f t="shared" si="4"/>
         <v>20152</v>
       </c>
       <c r="I47">
-        <f>(F47*1.1)</f>
+        <f t="shared" si="5"/>
         <v>20738.300000000003</v>
       </c>
       <c r="J47">
-        <f>(G47*2)</f>
+        <f t="shared" si="7"/>
         <v>1770</v>
       </c>
       <c r="K47">
-        <f>SUM(H47:J47)</f>
+        <f t="shared" si="6"/>
         <v>42660.3</v>
       </c>
       <c r="L47">
@@ -6608,19 +6608,19 @@
         <v>0</v>
       </c>
       <c r="H48">
-        <f>(E48*1.1)</f>
+        <f t="shared" si="4"/>
         <v>325559.30000000005</v>
       </c>
       <c r="I48">
-        <f>(F48*1.1)</f>
+        <f t="shared" si="5"/>
         <v>230972.50000000003</v>
       </c>
       <c r="J48">
-        <f>(G48*2)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K48">
-        <f>SUM(H48:J48)</f>
+        <f t="shared" si="6"/>
         <v>556531.80000000005</v>
       </c>
       <c r="L48">
@@ -6665,19 +6665,19 @@
         <v>8028</v>
       </c>
       <c r="H49">
-        <f>(E49*1.1)</f>
+        <f t="shared" si="4"/>
         <v>235516.6</v>
       </c>
       <c r="I49">
-        <f>(F49*1.1)</f>
+        <f t="shared" si="5"/>
         <v>166131.90000000002</v>
       </c>
       <c r="J49">
-        <f>(G49*2)</f>
+        <f t="shared" si="7"/>
         <v>16056</v>
       </c>
       <c r="K49">
-        <f>SUM(H49:J49)</f>
+        <f t="shared" si="6"/>
         <v>417704.5</v>
       </c>
       <c r="L49">
@@ -6722,19 +6722,19 @@
         <v>5283</v>
       </c>
       <c r="H50">
-        <f>(E50*1.1)</f>
+        <f t="shared" si="4"/>
         <v>101336.40000000001</v>
       </c>
       <c r="I50">
-        <f>(F50*1.1)</f>
+        <f t="shared" si="5"/>
         <v>89215.5</v>
       </c>
       <c r="J50">
-        <f>(G50*2)</f>
+        <f t="shared" si="7"/>
         <v>10566</v>
       </c>
       <c r="K50">
-        <f>SUM(H50:J50)</f>
+        <f t="shared" si="6"/>
         <v>201117.90000000002</v>
       </c>
       <c r="L50">
@@ -6779,19 +6779,19 @@
         <v>523</v>
       </c>
       <c r="H51">
-        <f>(E51*1.1)</f>
+        <f t="shared" si="4"/>
         <v>204930.00000000003</v>
       </c>
       <c r="I51">
-        <f>(F51*1.1)</f>
+        <f t="shared" si="5"/>
         <v>175762.40000000002</v>
       </c>
       <c r="J51">
-        <f>(G51*2)</f>
+        <f t="shared" si="7"/>
         <v>1046</v>
       </c>
       <c r="K51">
-        <f>SUM(H51:J51)</f>
+        <f t="shared" si="6"/>
         <v>381738.4</v>
       </c>
       <c r="L51">
@@ -6836,19 +6836,19 @@
         <v>1295</v>
       </c>
       <c r="H52">
-        <f>(E52*1.1)</f>
+        <f t="shared" si="4"/>
         <v>24825.9</v>
       </c>
       <c r="I52">
-        <f>(F52*1.1)</f>
+        <f t="shared" si="5"/>
         <v>28396.500000000004</v>
       </c>
       <c r="J52">
-        <f>(G52*2)</f>
+        <f t="shared" si="7"/>
         <v>2590</v>
       </c>
       <c r="K52">
-        <f>SUM(H52:J52)</f>
+        <f t="shared" si="6"/>
         <v>55812.400000000009</v>
       </c>
       <c r="L52">

</xml_diff>